<commit_message>
updating tests and gait data for slightly adjusted resampling method that should be more stable
</commit_message>
<xml_diff>
--- a/tests/gait/data/manual_gait_results_apcwt.xlsx
+++ b/tests/gait/data/manual_gait_results_apcwt.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lukasadamowicz/Documents/Packages/scikit-digital-health/test/gait/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lukasadamowicz/Documents/Packages/scikit-digital-health/tests/gait/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25532FA6-7C37-0444-B171-A23E190CEA82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DC270CE-161D-E34B-B9D4-0906574E3327}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="31720" windowHeight="24660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -724,9 +724,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -764,7 +764,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -870,7 +870,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1012,7 +1012,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1022,8 +1022,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AG82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J28" workbookViewId="0">
-      <selection activeCell="AB53" sqref="AB53:AB81"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="I52" sqref="I52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1164,13 +1164,13 @@
         <v>-1</v>
       </c>
       <c r="M2">
-        <v>0.16185390573236899</v>
+        <v>0.16184946556368701</v>
       </c>
       <c r="N2">
-        <v>4.0521976374824902E-2</v>
+        <v>4.0517453174439763E-2</v>
       </c>
       <c r="O2">
-        <v>2.4618477557035501E-2</v>
+        <v>2.461457757066653E-2</v>
       </c>
       <c r="P2">
         <v>0.99639999999999995</v>
@@ -1229,15 +1229,15 @@
       </c>
       <c r="AD2">
         <f>2 * SQRT(2 * P2 * N2 - N2 * N2) + 2 * SQRT(2 * AC2 * O2 - O2 * O2)</f>
-        <v>0.85222144820780854</v>
+        <v>0.85216841907780883</v>
       </c>
       <c r="AE2">
         <f>AD2+AD3</f>
-        <v>1.5870037139405293</v>
+        <v>1.5868897299706488</v>
       </c>
       <c r="AF2">
         <f>AE2/R2</f>
-        <v>1.3449184016445164</v>
+        <v>1.3448218050598719</v>
       </c>
       <c r="AG2">
         <f>60/Q2</f>
@@ -1279,13 +1279,13 @@
         <v>-1</v>
       </c>
       <c r="M3">
-        <v>0.14498481074516001</v>
+        <v>0.14497891099146051</v>
       </c>
       <c r="N3">
-        <v>3.7599078178544798E-2</v>
+        <v>3.7595195844124837E-2</v>
       </c>
       <c r="O3">
-        <v>1.06974112207748E-2</v>
+        <v>1.06936424492549E-2</v>
       </c>
       <c r="P3">
         <v>0.99639999999999995</v>
@@ -1344,15 +1344,15 @@
       </c>
       <c r="AD3">
         <f t="shared" ref="AD3:AD66" si="13">2 * SQRT(2 * P3 * N3 - N3 * N3) + 2 * SQRT(2 * AC3 * O3 - O3 * O3)</f>
-        <v>0.73478226573272076</v>
+        <v>0.73472131089283998</v>
       </c>
       <c r="AE3">
         <f t="shared" ref="AE3:AE66" si="14">AD3+AD4</f>
-        <v>1.4717247312446835</v>
+        <v>1.4716012138875763</v>
       </c>
       <c r="AF3">
         <f t="shared" ref="AF3:AF66" si="15">AE3/R3</f>
-        <v>1.3140399386113244</v>
+        <v>1.3139296552567643</v>
       </c>
       <c r="AG3">
         <f t="shared" ref="AG3:AG66" si="16">60/Q3</f>
@@ -1394,13 +1394,13 @@
         <v>-1</v>
       </c>
       <c r="M4">
-        <v>0.13006204280547301</v>
+        <v>0.1300495142745681</v>
       </c>
       <c r="N4">
-        <v>3.4302880315169197E-2</v>
+        <v>3.4298946516901747E-2</v>
       </c>
       <c r="O4">
-        <v>1.38370171540988E-2</v>
+        <v>1.383272471743659E-2</v>
       </c>
       <c r="P4">
         <v>0.99639999999999995</v>
@@ -1459,15 +1459,15 @@
       </c>
       <c r="AD4">
         <f t="shared" si="13"/>
-        <v>0.73694246551196285</v>
+        <v>0.73687990299473616</v>
       </c>
       <c r="AE4">
         <f t="shared" si="14"/>
-        <v>1.4445478743900666</v>
+        <v>1.4445436992698699</v>
       </c>
       <c r="AF4">
         <f t="shared" si="15"/>
-        <v>1.3132253403546059</v>
+        <v>1.3132215447907907</v>
       </c>
       <c r="AG4">
         <f t="shared" si="16"/>
@@ -1509,13 +1509,13 @@
         <v>-1</v>
       </c>
       <c r="M5">
-        <v>0.10894844966523901</v>
+        <v>0.10893148533430989</v>
       </c>
       <c r="N5">
-        <v>3.5251672674202303E-2</v>
+        <v>3.5256491115361763E-2</v>
       </c>
       <c r="O5">
-        <v>9.5718005077248796E-3</v>
+        <v>9.5742576122780382E-3</v>
       </c>
       <c r="P5">
         <v>0.99639999999999995</v>
@@ -1574,15 +1574,15 @@
       </c>
       <c r="AD5">
         <f t="shared" si="13"/>
-        <v>0.70760540887810386</v>
+        <v>0.70766379627513365</v>
       </c>
       <c r="AE5">
         <f t="shared" si="14"/>
-        <v>1.4676884000151618</v>
+        <v>1.4676826567602568</v>
       </c>
       <c r="AF5">
         <f t="shared" si="15"/>
-        <v>1.3342621818319651</v>
+        <v>1.3342569606911425</v>
       </c>
       <c r="AG5">
         <f t="shared" si="16"/>
@@ -1624,13 +1624,13 @@
         <v>-1</v>
       </c>
       <c r="M6">
-        <v>0.13959574254033599</v>
+        <v>0.13958610968651711</v>
       </c>
       <c r="N6">
-        <v>3.5816965743015503E-2</v>
+        <v>3.5813253369698123E-2</v>
       </c>
       <c r="O6">
-        <v>1.5430497607318801E-2</v>
+        <v>1.54254295841379E-2</v>
       </c>
       <c r="P6">
         <v>0.99639999999999995</v>
@@ -1689,15 +1689,15 @@
       </c>
       <c r="AD6">
         <f t="shared" si="13"/>
-        <v>0.76008299113705791</v>
+        <v>0.76001886048512313</v>
       </c>
       <c r="AE6">
         <f t="shared" si="14"/>
-        <v>1.5798631122162623</v>
+        <v>1.5797454615651998</v>
       </c>
       <c r="AF6">
         <f t="shared" si="15"/>
-        <v>1.3858448352774231</v>
+        <v>1.3857416329519299</v>
       </c>
       <c r="AG6">
         <f t="shared" si="16"/>
@@ -1739,13 +1739,13 @@
         <v>-1</v>
       </c>
       <c r="M7">
-        <v>0.13489147725195599</v>
+        <v>0.13488160989343051</v>
       </c>
       <c r="N7">
-        <v>4.5922036583071799E-2</v>
+        <v>4.5917860395715583E-2</v>
       </c>
       <c r="O7">
-        <v>1.42540981233028E-2</v>
+        <v>1.425057326042063E-2</v>
       </c>
       <c r="P7">
         <v>0.99639999999999995</v>
@@ -1804,15 +1804,15 @@
       </c>
       <c r="AD7">
         <f t="shared" si="13"/>
-        <v>0.81978012107920439</v>
+        <v>0.81972660108007678</v>
       </c>
       <c r="AE7">
         <f t="shared" si="14"/>
-        <v>1.5642131293289032</v>
+        <v>1.5641602954481773</v>
       </c>
       <c r="AF7">
         <f t="shared" si="15"/>
-        <v>1.3966188654722349</v>
+        <v>1.3965716923644438</v>
       </c>
       <c r="AG7">
         <f t="shared" si="16"/>
@@ -1854,13 +1854,13 @@
         <v>-1</v>
       </c>
       <c r="M8">
-        <v>0.132391438779659</v>
+        <v>0.13237418161142339</v>
       </c>
       <c r="N8">
-        <v>3.7986450333940901E-2</v>
+        <v>3.7981014312328511E-2</v>
       </c>
       <c r="O8">
-        <v>1.1490628383665999E-2</v>
+        <v>1.1495174758144801E-2</v>
       </c>
       <c r="P8">
         <v>0.99639999999999995</v>
@@ -1919,15 +1919,15 @@
       </c>
       <c r="AD8">
         <f t="shared" si="13"/>
-        <v>0.74443300824969871</v>
+        <v>0.74443369436810047</v>
       </c>
       <c r="AE8">
         <f t="shared" si="14"/>
-        <v>1.4927482867180277</v>
+        <v>1.4926701356299723</v>
       </c>
       <c r="AF8">
         <f t="shared" si="15"/>
-        <v>1.4082531006773846</v>
+        <v>1.4081793732358228</v>
       </c>
       <c r="AG8">
         <f t="shared" si="16"/>
@@ -1969,13 +1969,13 @@
         <v>-1</v>
       </c>
       <c r="M9">
-        <v>0.12873133206543699</v>
+        <v>0.12871432377491049</v>
       </c>
       <c r="N9">
-        <v>3.69436991270169E-2</v>
+        <v>3.6938791972117753E-2</v>
       </c>
       <c r="O9">
-        <v>1.2846284915476999E-2</v>
+        <v>1.284086338555481E-2</v>
       </c>
       <c r="P9">
         <v>0.99639999999999995</v>
@@ -2034,15 +2034,15 @@
       </c>
       <c r="AD9">
         <f t="shared" si="13"/>
-        <v>0.74831527846832901</v>
+        <v>0.74823644126187183</v>
       </c>
       <c r="AE9">
         <f t="shared" si="14"/>
-        <v>1.5633469722282132</v>
+        <v>1.5632068418828462</v>
       </c>
       <c r="AF9">
         <f t="shared" si="15"/>
-        <v>1.4748556341775596</v>
+        <v>1.4747234357385341</v>
       </c>
       <c r="AG9">
         <f t="shared" si="16"/>
@@ -2084,13 +2084,13 @@
         <v>-1</v>
       </c>
       <c r="M10">
-        <v>0.154134856492459</v>
+        <v>0.15412169514734539</v>
       </c>
       <c r="N10">
-        <v>4.1864748275934803E-2</v>
+        <v>4.1861258774164418E-2</v>
       </c>
       <c r="O10">
-        <v>1.7237665257267401E-2</v>
+        <v>1.7232176933011691E-2</v>
       </c>
       <c r="P10">
         <v>0.99639999999999995</v>
@@ -2149,15 +2149,15 @@
       </c>
       <c r="AD10">
         <f t="shared" si="13"/>
-        <v>0.81503169375988416</v>
+        <v>0.81497040062097448</v>
       </c>
       <c r="AE10">
         <f t="shared" si="14"/>
-        <v>1.607842338031245</v>
+        <v>1.6077045629867324</v>
       </c>
       <c r="AF10">
         <f t="shared" si="15"/>
-        <v>1.4887429055844861</v>
+        <v>1.4886153360988261</v>
       </c>
       <c r="AG10">
         <f t="shared" si="16"/>
@@ -2199,13 +2199,13 @@
         <v>-1</v>
       </c>
       <c r="M11">
-        <v>0.13157028678924601</v>
+        <v>0.1315586023181286</v>
       </c>
       <c r="N11">
-        <v>4.2680386542926302E-2</v>
+        <v>4.2674932730070128E-2</v>
       </c>
       <c r="O11">
-        <v>1.3486730317479901E-2</v>
+        <v>1.348159843515555E-2</v>
       </c>
       <c r="P11">
         <v>0.99639999999999995</v>
@@ -2264,15 +2264,15 @@
       </c>
       <c r="AD11">
         <f t="shared" si="13"/>
-        <v>0.79281064427136072</v>
+        <v>0.79273416236575778</v>
       </c>
       <c r="AE11">
         <f t="shared" si="14"/>
-        <v>1.6082041788579979</v>
+        <v>1.6080545970138747</v>
       </c>
       <c r="AF11">
         <f t="shared" si="15"/>
-        <v>1.4890779433870349</v>
+        <v>1.4889394416795134</v>
       </c>
       <c r="AG11">
         <f t="shared" si="16"/>
@@ -2314,13 +2314,13 @@
         <v>-1</v>
       </c>
       <c r="M12">
-        <v>0.151942612409662</v>
+        <v>0.1519279392143241</v>
       </c>
       <c r="N12">
-        <v>4.2585745691826798E-2</v>
+        <v>4.2581480655528872E-2</v>
       </c>
       <c r="O12">
-        <v>1.6603445720465501E-2</v>
+        <v>1.6597090358147819E-2</v>
       </c>
       <c r="P12">
         <v>0.99639999999999995</v>
@@ -2379,15 +2379,15 @@
       </c>
       <c r="AD12">
         <f t="shared" si="13"/>
-        <v>0.81539353458663733</v>
+        <v>0.81532043464811688</v>
       </c>
       <c r="AE12">
         <f t="shared" si="14"/>
-        <v>1.6205559325400385</v>
+        <v>1.6204061103347764</v>
       </c>
       <c r="AF12">
         <f t="shared" si="15"/>
-        <v>1.5582268582115755</v>
+        <v>1.5580827983988235</v>
       </c>
       <c r="AG12">
         <f t="shared" si="16"/>
@@ -2429,13 +2429,13 @@
         <v>-1</v>
       </c>
       <c r="M13">
-        <v>0.149187462117332</v>
+        <v>0.1491732516178641</v>
       </c>
       <c r="N13">
-        <v>3.9268916126777E-2</v>
+        <v>3.9265302612071798E-2</v>
       </c>
       <c r="O13">
-        <v>1.83794320481128E-2</v>
+        <v>1.837169554070469E-2</v>
       </c>
       <c r="P13">
         <v>0.99639999999999995</v>
@@ -2494,15 +2494,15 @@
       </c>
       <c r="AD13">
         <f t="shared" si="13"/>
-        <v>0.80516239795340128</v>
+        <v>0.80508567568665956</v>
       </c>
       <c r="AE13">
         <f t="shared" si="14"/>
-        <v>1.7244855689503273</v>
+        <v>1.7243270544014386</v>
       </c>
       <c r="AF13">
         <f t="shared" si="15"/>
-        <v>1.5967458971762289</v>
+        <v>1.5965991244457765</v>
       </c>
       <c r="AG13">
         <f t="shared" si="16"/>
@@ -2544,13 +2544,13 @@
         <v>-1</v>
       </c>
       <c r="M14">
-        <v>0.15018771299353501</v>
+        <v>0.15017414146491589</v>
       </c>
       <c r="N14">
-        <v>5.0001585747326799E-2</v>
+        <v>4.9994727741612392E-2</v>
       </c>
       <c r="O14">
-        <v>2.5730448063681601E-2</v>
+        <v>2.5723251306142308E-2</v>
       </c>
       <c r="P14">
         <v>0.99639999999999995</v>
@@ -2609,15 +2609,15 @@
       </c>
       <c r="AD14">
         <f t="shared" si="13"/>
-        <v>0.91932317099692618</v>
+        <v>0.91924137871477907</v>
       </c>
       <c r="AE14">
         <f t="shared" si="14"/>
-        <v>1.7248467673568815</v>
+        <v>1.7246926452896831</v>
       </c>
       <c r="AF14">
         <f t="shared" si="15"/>
-        <v>1.5970803401452605</v>
+        <v>1.5969376345274844</v>
       </c>
       <c r="AG14">
         <f t="shared" si="16"/>
@@ -2659,13 +2659,13 @@
         <v>-1</v>
       </c>
       <c r="M15">
-        <v>0.14059351689439301</v>
+        <v>0.14058129264802111</v>
       </c>
       <c r="N15">
-        <v>3.9727835627711698E-2</v>
+        <v>3.9724729572057117E-2</v>
       </c>
       <c r="O15">
-        <v>1.79631898365658E-2</v>
+        <v>1.795565836035309E-2</v>
       </c>
       <c r="P15">
         <v>0.99639999999999995</v>
@@ -2724,15 +2724,15 @@
       </c>
       <c r="AD15">
         <f t="shared" si="13"/>
-        <v>0.80552359635995541</v>
+        <v>0.80545126657490407</v>
       </c>
       <c r="AE15">
         <f t="shared" si="14"/>
-        <v>1.7017971353791099</v>
+        <v>1.7016563497106918</v>
       </c>
       <c r="AF15">
         <f t="shared" si="15"/>
-        <v>1.5470883048900999</v>
+        <v>1.5469603179188105</v>
       </c>
       <c r="AG15">
         <f t="shared" si="16"/>
@@ -2774,13 +2774,13 @@
         <v>-1</v>
       </c>
       <c r="M16">
-        <v>0.157195403946672</v>
+        <v>0.15719317053664569</v>
       </c>
       <c r="N16">
-        <v>4.9086185561815598E-2</v>
+        <v>4.9081880396406527E-2</v>
       </c>
       <c r="O16">
-        <v>2.2702958870976599E-2</v>
+        <v>2.269591694243921E-2</v>
       </c>
       <c r="P16">
         <v>0.99639999999999995</v>
@@ -2839,15 +2839,15 @@
       </c>
       <c r="AD16">
         <f t="shared" si="13"/>
-        <v>0.89627353901915452</v>
+        <v>0.89620508313578773</v>
       </c>
       <c r="AE16">
         <f t="shared" si="14"/>
-        <v>1.5928120971217805</v>
+        <v>1.5926561506396877</v>
       </c>
       <c r="AF16">
         <f t="shared" si="15"/>
-        <v>1.4221536581444467</v>
+        <v>1.4220144202140068</v>
       </c>
       <c r="AG16">
         <f t="shared" si="16"/>
@@ -2889,13 +2889,13 @@
         <v>-1</v>
       </c>
       <c r="M17">
-        <v>0.13474243492186899</v>
+        <v>0.134731872421745</v>
       </c>
       <c r="N17">
-        <v>3.1994040275593702E-2</v>
+        <v>3.1987971745841157E-2</v>
       </c>
       <c r="O17">
-        <v>1.1047945170094799E-2</v>
+        <v>1.1043282312708029E-2</v>
       </c>
       <c r="P17">
         <v>0.99639999999999995</v>
@@ -2954,15 +2954,15 @@
       </c>
       <c r="AD17">
         <f t="shared" si="13"/>
-        <v>0.69653855810262599</v>
+        <v>0.69645106750389996</v>
       </c>
       <c r="AE17">
         <f t="shared" si="14"/>
-        <v>1.619195014171962</v>
+        <v>1.6190386477258589</v>
       </c>
       <c r="AF17">
         <f t="shared" si="15"/>
-        <v>1.4203465036596159</v>
+        <v>1.4202093401104028</v>
       </c>
       <c r="AG17">
         <f t="shared" si="16"/>
@@ -3004,13 +3004,13 @@
         <v>-1</v>
       </c>
       <c r="M18">
-        <v>0.17509429580993699</v>
+        <v>0.17510075727623431</v>
       </c>
       <c r="N18">
-        <v>4.96705315533E-2</v>
+        <v>4.9665843307315542E-2</v>
       </c>
       <c r="O18">
-        <v>2.6698993641145599E-2</v>
+        <v>2.6691620546169161E-2</v>
       </c>
       <c r="P18">
         <v>0.99639999999999995</v>
@@ -3069,15 +3069,15 @@
       </c>
       <c r="AD18">
         <f t="shared" si="13"/>
-        <v>0.922656456069336</v>
+        <v>0.92258758022195897</v>
       </c>
       <c r="AE18">
         <f t="shared" si="14"/>
-        <v>1.6149824206554855</v>
+        <v>1.6149445475483994</v>
       </c>
       <c r="AF18">
         <f t="shared" si="15"/>
-        <v>1.3237560825044963</v>
+        <v>1.323725038974098</v>
       </c>
       <c r="AG18">
         <f t="shared" si="16"/>
@@ -3119,13 +3119,13 @@
         <v>-1</v>
       </c>
       <c r="M19">
-        <v>0.14314849059799201</v>
+        <v>0.14314803487239089</v>
       </c>
       <c r="N19">
-        <v>3.3347314815691198E-2</v>
+        <v>3.3344683224733107E-2</v>
       </c>
       <c r="O19">
-        <v>9.4511102849159992E-3</v>
+        <v>9.4564756178791842E-3</v>
       </c>
       <c r="P19">
         <v>0.99639999999999995</v>
@@ -3184,15 +3184,15 @@
       </c>
       <c r="AD19">
         <f t="shared" si="13"/>
-        <v>0.69232596458614948</v>
+        <v>0.69235696732644048</v>
       </c>
       <c r="AE19">
         <f t="shared" si="14"/>
-        <v>1.3588421142300073</v>
+        <v>1.3589682103347598</v>
       </c>
       <c r="AF19">
         <f t="shared" si="15"/>
-        <v>1.1919667668684275</v>
+        <v>1.1920773774866316</v>
       </c>
       <c r="AG19">
         <f t="shared" si="16"/>
@@ -3234,13 +3234,13 @@
         <v>-1</v>
       </c>
       <c r="M20">
-        <v>0.10294474236567799</v>
+        <v>0.10292354735372861</v>
       </c>
       <c r="N20">
-        <v>3.24005946715408E-2</v>
+        <v>3.2407114399682371E-2</v>
       </c>
       <c r="O20">
-        <v>7.5909055781966904E-3</v>
+        <v>7.5951692488158574E-3</v>
       </c>
       <c r="P20">
         <v>0.99639999999999995</v>
@@ -3299,15 +3299,15 @@
       </c>
       <c r="AD20">
         <f t="shared" si="13"/>
-        <v>0.66651614964385786</v>
+        <v>0.6666112430083192</v>
       </c>
       <c r="AE20">
         <f t="shared" si="14"/>
-        <v>1.4383575932403949</v>
+        <v>1.4384472734061844</v>
       </c>
       <c r="AF20">
         <f t="shared" si="15"/>
-        <v>1.3075978120367227</v>
+        <v>1.3076793394601676</v>
       </c>
       <c r="AG20">
         <f t="shared" si="16"/>
@@ -3349,13 +3349,13 @@
         <v>-1</v>
       </c>
       <c r="M21">
-        <v>0.128390848859361</v>
+        <v>0.12836843662188449</v>
       </c>
       <c r="N21">
-        <v>4.0895973840902197E-2</v>
+        <v>4.0888934857715463E-2</v>
       </c>
       <c r="O21">
-        <v>1.2364815382203499E-2</v>
+        <v>1.2369936096812849E-2</v>
       </c>
       <c r="P21">
         <v>0.99639999999999995</v>
@@ -3414,15 +3414,15 @@
       </c>
       <c r="AD21">
         <f t="shared" si="13"/>
-        <v>0.77184144359653706</v>
+        <v>0.77183603039786519</v>
       </c>
       <c r="AE21">
         <f t="shared" si="14"/>
-        <v>1.4746170679096033</v>
+        <v>1.4746024648799048</v>
       </c>
       <c r="AF21">
         <f t="shared" si="15"/>
-        <v>1.3405609708269119</v>
+        <v>1.3405476953453679</v>
       </c>
       <c r="AG21">
         <f t="shared" si="16"/>
@@ -3464,13 +3464,13 @@
         <v>-1</v>
       </c>
       <c r="M22">
-        <v>0.11390645310112101</v>
+        <v>0.1138955614064207</v>
       </c>
       <c r="N22">
-        <v>3.3950006855465099E-2</v>
+        <v>3.3955343959704898E-2</v>
       </c>
       <c r="O22">
-        <v>1.0087626127212399E-2</v>
+        <v>1.0082275580157739E-2</v>
       </c>
       <c r="P22">
         <v>0.99639999999999995</v>
@@ -3529,15 +3529,15 @@
       </c>
       <c r="AD22">
         <f t="shared" si="13"/>
-        <v>0.70277562431306628</v>
+        <v>0.70276643448203968</v>
       </c>
       <c r="AE22">
         <f t="shared" si="14"/>
-        <v>1.4337029425805627</v>
+        <v>1.4337006581518457</v>
       </c>
       <c r="AF22">
         <f t="shared" si="15"/>
-        <v>1.327502724611632</v>
+        <v>1.3275006093998569</v>
       </c>
       <c r="AG22">
         <f t="shared" si="16"/>
@@ -3579,13 +3579,13 @@
         <v>-1</v>
       </c>
       <c r="M23">
-        <v>0.125036409412984</v>
+        <v>0.12501936485641349</v>
       </c>
       <c r="N23">
-        <v>3.7586332774979601E-2</v>
+        <v>3.7579890332483282E-2</v>
       </c>
       <c r="O23">
-        <v>1.0278130132952999E-2</v>
+        <v>1.0283915060627889E-2</v>
       </c>
       <c r="P23">
         <v>0.99639999999999995</v>
@@ -3644,15 +3644,15 @@
       </c>
       <c r="AD23">
         <f t="shared" si="13"/>
-        <v>0.73092731826749635</v>
+        <v>0.73093422366980598</v>
       </c>
       <c r="AE23">
         <f t="shared" si="14"/>
-        <v>1.4867608135409596</v>
+        <v>1.4866675911629637</v>
       </c>
       <c r="AF23">
         <f t="shared" si="15"/>
-        <v>1.3766303829082958</v>
+        <v>1.376544065891633</v>
       </c>
       <c r="AG23">
         <f t="shared" si="16"/>
@@ -3694,13 +3694,13 @@
         <v>-1</v>
       </c>
       <c r="M24">
-        <v>0.13598326181440201</v>
+        <v>0.13597290545639229</v>
       </c>
       <c r="N24">
-        <v>3.6369279889507999E-2</v>
+        <v>3.6362859206698378E-2</v>
       </c>
       <c r="O24">
-        <v>1.43288836166044E-2</v>
+        <v>1.43218186892991E-2</v>
       </c>
       <c r="P24">
         <v>0.99639999999999995</v>
@@ -3759,15 +3759,15 @@
       </c>
       <c r="AD24">
         <f t="shared" si="13"/>
-        <v>0.75583349527346322</v>
+        <v>0.75573336749315767</v>
       </c>
       <c r="AE24">
         <f t="shared" si="14"/>
-        <v>1.4845092232630601</v>
+        <v>1.4843145891976819</v>
       </c>
       <c r="AF24">
         <f t="shared" si="15"/>
-        <v>1.374545577095426</v>
+        <v>1.374365360368224</v>
       </c>
       <c r="AG24">
         <f t="shared" si="16"/>
@@ -3809,13 +3809,13 @@
         <v>-1</v>
       </c>
       <c r="M25">
-        <v>0.13396215822336</v>
+        <v>0.13394765940530759</v>
       </c>
       <c r="N25">
-        <v>3.3568185820871101E-2</v>
+        <v>3.3562817186396227E-2</v>
       </c>
       <c r="O25">
-        <v>1.34815040251249E-2</v>
+        <v>1.347462557941128E-2</v>
       </c>
       <c r="P25">
         <v>0.99639999999999995</v>
@@ -3874,15 +3874,15 @@
       </c>
       <c r="AD25">
         <f t="shared" si="13"/>
-        <v>0.72867572798959679</v>
+        <v>0.72858122170452422</v>
       </c>
       <c r="AE25">
         <f t="shared" si="14"/>
-        <v>1.5189147665042733</v>
+        <v>1.5187247833488724</v>
       </c>
       <c r="AF25">
         <f t="shared" si="15"/>
-        <v>1.3561738986645295</v>
+        <v>1.3560042708472073</v>
       </c>
       <c r="AG25">
         <f t="shared" si="16"/>
@@ -3924,13 +3924,13 @@
         <v>-1</v>
       </c>
       <c r="M26">
-        <v>0.14826987791787299</v>
+        <v>0.1482609007370117</v>
       </c>
       <c r="N26">
-        <v>3.7907536911037203E-2</v>
+        <v>3.7902196835692577E-2</v>
       </c>
       <c r="O26">
-        <v>1.75776192328388E-2</v>
+        <v>1.7569170346108661E-2</v>
       </c>
       <c r="P26">
         <v>0.99639999999999995</v>
@@ -3989,15 +3989,15 @@
       </c>
       <c r="AD26">
         <f t="shared" si="13"/>
-        <v>0.79023903851467647</v>
+        <v>0.79014356164434818</v>
       </c>
       <c r="AE26">
         <f t="shared" si="14"/>
-        <v>1.5384107772724693</v>
+        <v>1.5382138018277123</v>
       </c>
       <c r="AF26">
         <f t="shared" si="15"/>
-        <v>1.3262161873038529</v>
+        <v>1.3260463808859591</v>
       </c>
       <c r="AG26">
         <f t="shared" si="16"/>
@@ -4039,13 +4039,13 @@
         <v>-1</v>
       </c>
       <c r="M27">
-        <v>0.13526015700060801</v>
+        <v>0.13524637380887361</v>
       </c>
       <c r="N27">
-        <v>4.0901995757580897E-2</v>
+        <v>4.0894654780033131E-2</v>
       </c>
       <c r="O27">
-        <v>9.6614915547132592E-3</v>
+        <v>9.6559581249134989E-3</v>
       </c>
       <c r="P27">
         <v>0.99639999999999995</v>
@@ -4104,15 +4104,15 @@
       </c>
       <c r="AD27">
         <f t="shared" si="13"/>
-        <v>0.74817173875779286</v>
+        <v>0.7480702401833641</v>
       </c>
       <c r="AE27">
         <f t="shared" si="14"/>
-        <v>1.4151728489710891</v>
+        <v>1.4150680114053111</v>
       </c>
       <c r="AF27">
         <f t="shared" si="15"/>
-        <v>1.2635471865813295</v>
+        <v>1.2634535816118848</v>
       </c>
       <c r="AG27">
         <f t="shared" si="16"/>
@@ -4154,13 +4154,13 @@
         <v>-1</v>
       </c>
       <c r="M28">
-        <v>0.11350456325432599</v>
+        <v>0.11350168889525029</v>
       </c>
       <c r="N28">
-        <v>2.9335092176505501E-2</v>
+        <v>2.9341722360078541E-2</v>
       </c>
       <c r="O28">
-        <v>1.0087129538600199E-2</v>
+        <v>1.008093427855155E-2</v>
       </c>
       <c r="P28">
         <v>0.99639999999999995</v>
@@ -4219,15 +4219,15 @@
       </c>
       <c r="AD28">
         <f t="shared" si="13"/>
-        <v>0.66700111021329611</v>
+        <v>0.66699777122194703</v>
       </c>
       <c r="AE28">
         <f t="shared" si="14"/>
-        <v>1.416927645448419</v>
+        <v>1.4169422291808889</v>
       </c>
       <c r="AF28">
         <f t="shared" si="15"/>
-        <v>1.2429189872354554</v>
+        <v>1.242931779983236</v>
       </c>
       <c r="AG28">
         <f t="shared" si="16"/>
@@ -4269,13 +4269,13 @@
         <v>-1</v>
       </c>
       <c r="M29">
-        <v>0.13654921191365099</v>
+        <v>0.1365323490014923</v>
       </c>
       <c r="N29">
-        <v>3.6769437007087603E-2</v>
+        <v>3.6763028985371461E-2</v>
       </c>
       <c r="O29">
-        <v>1.3202439659863899E-2</v>
+        <v>1.321044970342404E-2</v>
       </c>
       <c r="P29">
         <v>0.99639999999999995</v>
@@ -4334,15 +4334,15 @@
       </c>
       <c r="AD29">
         <f t="shared" si="13"/>
-        <v>0.74992653523512276</v>
+        <v>0.74994445795894182</v>
       </c>
       <c r="AE29">
         <f t="shared" si="14"/>
-        <v>1.4519710896334477</v>
+        <v>1.4519901562399533</v>
       </c>
       <c r="AF29">
         <f t="shared" si="15"/>
-        <v>1.2304839742656337</v>
+        <v>1.2305001324067402</v>
       </c>
       <c r="AG29">
         <f t="shared" si="16"/>
@@ -4384,13 +4384,13 @@
         <v>-1</v>
       </c>
       <c r="M30">
-        <v>0.12255029511389599</v>
+        <v>0.1225449654837866</v>
       </c>
       <c r="N30">
-        <v>3.4114693913549397E-2</v>
+        <v>3.4122176448995678E-2</v>
       </c>
       <c r="O30">
-        <v>9.8749938821930498E-3</v>
+        <v>9.869104475158718E-3</v>
       </c>
       <c r="P30">
         <v>0.99639999999999995</v>
@@ -4449,15 +4449,15 @@
       </c>
       <c r="AD30">
         <f t="shared" si="13"/>
-        <v>0.70204455439832492</v>
+        <v>0.70204569828101149</v>
       </c>
       <c r="AE30">
         <f t="shared" si="14"/>
-        <v>1.3980253215770291</v>
+        <v>1.3980952688331927</v>
       </c>
       <c r="AF30">
         <f t="shared" si="15"/>
-        <v>1.2482368942652045</v>
+        <v>1.2482993471724932</v>
       </c>
       <c r="AG30">
         <f t="shared" si="16"/>
@@ -4499,13 +4499,13 @@
         <v>-1</v>
       </c>
       <c r="M31">
-        <v>0.11368222820110099</v>
+        <v>0.1136677400081261</v>
       </c>
       <c r="N31">
-        <v>3.5423445805113599E-2</v>
+        <v>3.5420682978659128E-2</v>
       </c>
       <c r="O31">
-        <v>8.2539531592621708E-3</v>
+        <v>8.2627117258748141E-3</v>
       </c>
       <c r="P31">
         <v>0.99639999999999995</v>
@@ -4564,15 +4564,15 @@
       </c>
       <c r="AD31">
         <f t="shared" si="13"/>
-        <v>0.69598076717870416</v>
+        <v>0.6960495705521812</v>
       </c>
       <c r="AE31">
         <f t="shared" si="14"/>
-        <v>1.4160259043734955</v>
+        <v>1.4159532262109569</v>
       </c>
       <c r="AF31">
         <f t="shared" si="15"/>
-        <v>1.3111350966421254</v>
+        <v>1.3110678020471822</v>
       </c>
       <c r="AG31">
         <f t="shared" si="16"/>
@@ -4614,13 +4614,13 @@
         <v>-1</v>
       </c>
       <c r="M32">
-        <v>0.121770203568181</v>
+        <v>0.1217374057222079</v>
       </c>
       <c r="N32">
-        <v>3.1812942158679802E-2</v>
+        <v>3.1803671455467489E-2</v>
       </c>
       <c r="O32">
-        <v>1.40896699834984E-2</v>
+        <v>1.408059421630878E-2</v>
       </c>
       <c r="P32">
         <v>0.99639999999999995</v>
@@ -4679,15 +4679,15 @@
       </c>
       <c r="AD32">
         <f t="shared" si="13"/>
-        <v>0.72004513719479135</v>
+        <v>0.71990365565877568</v>
       </c>
       <c r="AE32">
         <f t="shared" si="14"/>
-        <v>1.5119440550633048</v>
+        <v>1.5116994571160536</v>
       </c>
       <c r="AF32">
         <f t="shared" si="15"/>
-        <v>1.3744945955120951</v>
+        <v>1.3742722337418667</v>
       </c>
       <c r="AG32">
         <f t="shared" si="16"/>
@@ -4729,13 +4729,13 @@
         <v>-1</v>
       </c>
       <c r="M33">
-        <v>0.14047573151176901</v>
+        <v>0.1404560578924495</v>
       </c>
       <c r="N33">
-        <v>4.3323457392324398E-2</v>
+        <v>4.3316030754176657E-2</v>
       </c>
       <c r="O33">
-        <v>1.28415669265161E-2</v>
+        <v>1.2834835291764929E-2</v>
       </c>
       <c r="P33">
         <v>0.99639999999999995</v>
@@ -4794,15 +4794,15 @@
       </c>
       <c r="AD33">
         <f t="shared" si="13"/>
-        <v>0.7918989178685133</v>
+        <v>0.7917958014572779</v>
       </c>
       <c r="AE33">
         <f t="shared" si="14"/>
-        <v>1.5148491241645541</v>
+        <v>1.5146363360086381</v>
       </c>
       <c r="AF33">
         <f t="shared" si="15"/>
-        <v>1.3771355674223218</v>
+        <v>1.3769421236442163</v>
       </c>
       <c r="AG33">
         <f t="shared" si="16"/>
@@ -4844,13 +4844,13 @@
         <v>-1</v>
       </c>
       <c r="M34">
-        <v>0.13924549361417299</v>
+        <v>0.13922889564424029</v>
       </c>
       <c r="N34">
-        <v>3.2280197895042002E-2</v>
+        <v>3.2274470030863908E-2</v>
       </c>
       <c r="O34">
-        <v>1.40001626068781E-2</v>
+        <v>1.399164846499041E-2</v>
       </c>
       <c r="P34">
         <v>0.99639999999999995</v>
@@ -4909,15 +4909,15 @@
       </c>
       <c r="AD34">
         <f t="shared" si="13"/>
-        <v>0.72295020629604079</v>
+        <v>0.72284053455136021</v>
       </c>
       <c r="AE34">
         <f t="shared" si="14"/>
-        <v>1.5088306531413087</v>
+        <v>1.5086204850651257</v>
       </c>
       <c r="AF34">
         <f t="shared" si="15"/>
-        <v>1.3471702260190255</v>
+        <v>1.346982575951005</v>
       </c>
       <c r="AG34">
         <f t="shared" si="16"/>
@@ -4959,13 +4959,13 @@
         <v>-1</v>
       </c>
       <c r="M35">
-        <v>0.13691765413736501</v>
+        <v>0.1368963409588238</v>
       </c>
       <c r="N35">
-        <v>4.3215652485745798E-2</v>
+        <v>4.3209108351944928E-2</v>
       </c>
       <c r="O35">
-        <v>1.2193101353316801E-2</v>
+        <v>1.218617474586184E-2</v>
       </c>
       <c r="P35">
         <v>0.99639999999999995</v>
@@ -5024,15 +5024,15 @@
       </c>
       <c r="AD35">
         <f t="shared" si="13"/>
-        <v>0.78588044684526803</v>
+        <v>0.78577995051376548</v>
       </c>
       <c r="AE35">
         <f t="shared" si="14"/>
-        <v>1.4889849990462538</v>
+        <v>1.4887806813942652</v>
       </c>
       <c r="AF35">
         <f t="shared" si="15"/>
-        <v>1.3061271921458368</v>
+        <v>1.3059479661353204</v>
       </c>
       <c r="AG35">
         <f t="shared" si="16"/>
@@ -5074,13 +5074,13 @@
         <v>-1</v>
       </c>
       <c r="M36">
-        <v>0.13240148979685701</v>
+        <v>0.13239189233459531</v>
       </c>
       <c r="N36">
-        <v>2.99516475591044E-2</v>
+        <v>2.9947125836083621E-2</v>
       </c>
       <c r="O36">
-        <v>1.3787780551443699E-2</v>
+        <v>1.377907664035259E-2</v>
       </c>
       <c r="P36">
         <v>0.99639999999999995</v>
@@ -5139,15 +5139,15 @@
       </c>
       <c r="AD36">
         <f t="shared" si="13"/>
-        <v>0.70310455220098578</v>
+        <v>0.70300073088049975</v>
       </c>
       <c r="AE36">
         <f t="shared" si="14"/>
-        <v>1.4183262111942501</v>
+        <v>1.4181252153951098</v>
       </c>
       <c r="AF36">
         <f t="shared" si="15"/>
-        <v>1.2663626885662946</v>
+        <v>1.2661832280313479</v>
       </c>
       <c r="AG36">
         <f t="shared" si="16"/>
@@ -5189,13 +5189,13 @@
         <v>-1</v>
       </c>
       <c r="M37">
-        <v>0.118751406233884</v>
+        <v>0.1187272779568419</v>
       </c>
       <c r="N37">
-        <v>3.3193313854574698E-2</v>
+        <v>3.3187310783150653E-2</v>
       </c>
       <c r="O37">
-        <v>1.2167257819512599E-2</v>
+        <v>1.2161022739955439E-2</v>
       </c>
       <c r="P37">
         <v>0.99639999999999995</v>
@@ -5254,15 +5254,15 @@
       </c>
       <c r="AD37">
         <f t="shared" si="13"/>
-        <v>0.71522165899326418</v>
+        <v>0.71512448451461008</v>
       </c>
       <c r="AE37">
         <f t="shared" si="14"/>
-        <v>1.5345260629304556</v>
+        <v>1.5343464332224375</v>
       </c>
       <c r="AF37">
         <f t="shared" si="15"/>
-        <v>1.300445816042759</v>
+        <v>1.3002935874766419</v>
       </c>
       <c r="AG37">
         <f t="shared" si="16"/>
@@ -5304,13 +5304,13 @@
         <v>-1</v>
       </c>
       <c r="M38">
-        <v>0.158885784584713</v>
+        <v>0.15888728239521199</v>
       </c>
       <c r="N38">
-        <v>3.9894495441786401E-2</v>
+        <v>3.9889772499983218E-2</v>
       </c>
       <c r="O38">
-        <v>1.9881694801637199E-2</v>
+        <v>1.9873885631588609E-2</v>
       </c>
       <c r="P38">
         <v>0.99639999999999995</v>
@@ -5369,15 +5369,15 @@
       </c>
       <c r="AD38">
         <f t="shared" si="13"/>
-        <v>0.81930440393719128</v>
+        <v>0.81922194870782739</v>
       </c>
       <c r="AE38">
         <f t="shared" si="14"/>
-        <v>1.3997298891463963</v>
+        <v>1.3995901610426444</v>
       </c>
       <c r="AF38">
         <f t="shared" si="15"/>
-        <v>1.4282958052514247</v>
+        <v>1.4281532255537188</v>
       </c>
       <c r="AG38">
         <f t="shared" si="16"/>
@@ -5419,13 +5419,13 @@
         <v>-1</v>
       </c>
       <c r="M39">
-        <v>7.7597963914188606E-2</v>
+        <v>7.7612317388435825E-2</v>
       </c>
       <c r="N39">
-        <v>1.6631927333901599E-2</v>
+        <v>1.6632997071848801E-2</v>
       </c>
       <c r="O39">
-        <v>1.3745212035663999E-2</v>
+        <v>1.373638617245778E-2</v>
       </c>
       <c r="P39">
         <v>0.99639999999999995</v>
@@ -5484,15 +5484,15 @@
       </c>
       <c r="AD39">
         <f t="shared" si="13"/>
-        <v>0.58042548520920501</v>
+        <v>0.58036821233481706</v>
       </c>
       <c r="AE39">
         <f t="shared" si="14"/>
-        <v>1.046747767677024</v>
+        <v>1.0466250077460175</v>
       </c>
       <c r="AF39">
         <f t="shared" si="15"/>
-        <v>0.90236876523881393</v>
+        <v>0.9022629377120841</v>
       </c>
       <c r="AG39">
         <f t="shared" si="16"/>
@@ -5534,13 +5534,13 @@
         <v>-1</v>
       </c>
       <c r="M40">
-        <v>0.100557182310455</v>
+        <v>0.10051283278935701</v>
       </c>
       <c r="N40">
-        <v>1.3811596962731499E-2</v>
+        <v>1.38092454967666E-2</v>
       </c>
       <c r="O40">
-        <v>5.2796388169384801E-3</v>
+        <v>5.2767000328017427E-3</v>
       </c>
       <c r="P40">
         <v>0.99639999999999995</v>
@@ -5599,15 +5599,15 @@
       </c>
       <c r="AD40">
         <f t="shared" si="13"/>
-        <v>0.46632228246781915</v>
+        <v>0.46625679541120046</v>
       </c>
       <c r="AE40">
         <f t="shared" si="14"/>
-        <v>1.1152666134049478</v>
+        <v>1.115220202001789</v>
       </c>
       <c r="AF40">
         <f t="shared" si="15"/>
-        <v>0.68843618111416527</v>
+        <v>0.68840753209986971</v>
       </c>
       <c r="AG40">
         <f t="shared" si="16"/>
@@ -5649,13 +5649,13 @@
         <v>-1</v>
       </c>
       <c r="M41">
-        <v>2.2462897780411401E-2</v>
+        <v>2.2465498697180761E-2</v>
       </c>
       <c r="N41">
-        <v>3.5365781688139801E-2</v>
+        <v>3.5371424163704077E-2</v>
       </c>
       <c r="O41">
-        <v>4.3156487997151396E-3</v>
+        <v>4.3140839599347721E-3</v>
       </c>
       <c r="P41">
         <v>0.99639999999999995</v>
@@ -5714,15 +5714,15 @@
       </c>
       <c r="AD41">
         <f t="shared" si="13"/>
-        <v>0.64894433093712878</v>
+        <v>0.64896340659058838</v>
       </c>
       <c r="AE41">
         <f t="shared" si="14"/>
-        <v>1.4249866235194841</v>
+        <v>1.424992089811747</v>
       </c>
       <c r="AF41">
         <f t="shared" si="15"/>
-        <v>0.9760182352873179</v>
+        <v>0.97602197932311441</v>
       </c>
       <c r="AG41">
         <f t="shared" si="16"/>
@@ -5764,13 +5764,13 @@
         <v>-1</v>
       </c>
       <c r="M42">
-        <v>8.2769479429830706E-2</v>
+        <v>8.2749650998294594E-2</v>
       </c>
       <c r="N42">
-        <v>3.48913207415723E-2</v>
+        <v>3.4882431692045843E-2</v>
       </c>
       <c r="O42">
-        <v>1.8692339035480399E-2</v>
+        <v>1.8700154617452409E-2</v>
       </c>
       <c r="P42">
         <v>0.99639999999999995</v>
@@ -5829,15 +5829,15 @@
       </c>
       <c r="AD42">
         <f t="shared" si="13"/>
-        <v>0.77604229258235546</v>
+        <v>0.77602868322115859</v>
       </c>
       <c r="AE42">
         <f t="shared" si="14"/>
-        <v>1.4365874390987097</v>
+        <v>1.4366494232627327</v>
       </c>
       <c r="AF42">
         <f t="shared" si="15"/>
-        <v>1.158538257337669</v>
+        <v>1.1585882445667199</v>
       </c>
       <c r="AG42">
         <f t="shared" si="16"/>
@@ -5879,13 +5879,13 @@
         <v>-1</v>
       </c>
       <c r="M43">
-        <v>9.1766799383546593E-2</v>
+        <v>9.1753169158227288E-2</v>
       </c>
       <c r="N43">
-        <v>3.34176136723289E-2</v>
+        <v>3.3420185465695043E-2</v>
       </c>
       <c r="O43">
-        <v>6.3566335422469804E-3</v>
+        <v>6.3614755418905178E-3</v>
       </c>
       <c r="P43">
         <v>0.99639999999999995</v>
@@ -5944,15 +5944,15 @@
       </c>
       <c r="AD43">
         <f t="shared" si="13"/>
-        <v>0.66054514651635432</v>
+        <v>0.66062074004157412</v>
       </c>
       <c r="AE43">
         <f t="shared" si="14"/>
-        <v>1.3555629528514914</v>
+        <v>1.3557925953237411</v>
       </c>
       <c r="AF43">
         <f t="shared" si="15"/>
-        <v>1.1890903095188523</v>
+        <v>1.1892917502839835</v>
       </c>
       <c r="AG43">
         <f t="shared" si="16"/>
@@ -5994,13 +5994,13 @@
         <v>-1</v>
       </c>
       <c r="M44">
-        <v>9.1493956096193804E-2</v>
+        <v>9.1464396697055597E-2</v>
       </c>
       <c r="N44">
-        <v>3.36718006468089E-2</v>
+        <v>3.3680929131565791E-2</v>
       </c>
       <c r="O44">
-        <v>9.4778379906895003E-3</v>
+        <v>9.4868893323415988E-3</v>
       </c>
       <c r="P44">
         <v>0.99639999999999995</v>
@@ -6059,15 +6059,15 @@
       </c>
       <c r="AD44">
         <f t="shared" si="13"/>
-        <v>0.69501780633513699</v>
+        <v>0.69517185528216685</v>
       </c>
       <c r="AE44">
         <f t="shared" si="14"/>
-        <v>1.485952798344</v>
+        <v>1.4859983211067536</v>
       </c>
       <c r="AF44">
         <f t="shared" si="15"/>
-        <v>1.3267435699499999</v>
+        <v>1.3267842152738869</v>
       </c>
       <c r="AG44">
         <f t="shared" si="16"/>
@@ -6109,13 +6109,13 @@
         <v>-1</v>
       </c>
       <c r="M45">
-        <v>0.141213881148823</v>
+        <v>0.14120052720009829</v>
       </c>
       <c r="N45">
-        <v>3.9439750523496499E-2</v>
+        <v>3.9431517412599572E-2</v>
       </c>
       <c r="O45">
-        <v>1.61523164381637E-2</v>
+        <v>1.6145092114921201E-2</v>
       </c>
       <c r="P45">
         <v>0.99639999999999995</v>
@@ -6174,15 +6174,15 @@
       </c>
       <c r="AD45">
         <f t="shared" si="13"/>
-        <v>0.79093499200886286</v>
+        <v>0.7908264658245866</v>
       </c>
       <c r="AE45">
         <f t="shared" si="14"/>
-        <v>1.4926168647156861</v>
+        <v>1.4923610520849029</v>
       </c>
       <c r="AF45">
         <f t="shared" si="15"/>
-        <v>1.3326936292104339</v>
+        <v>1.332465225075806</v>
       </c>
       <c r="AG45">
         <f t="shared" si="16"/>
@@ -6224,13 +6224,13 @@
         <v>-1</v>
       </c>
       <c r="M46">
-        <v>0.13239726771552501</v>
+        <v>0.1323743419731431</v>
       </c>
       <c r="N46">
-        <v>3.3410114354889997E-2</v>
+        <v>3.3401007382373171E-2</v>
       </c>
       <c r="O46">
-        <v>1.0412639167956501E-2</v>
+        <v>1.0403905330022129E-2</v>
       </c>
       <c r="P46">
         <v>0.99639999999999995</v>
@@ -6289,15 +6289,15 @@
       </c>
       <c r="AD46">
         <f t="shared" si="13"/>
-        <v>0.70168187270682314</v>
+        <v>0.7015345862603164</v>
       </c>
       <c r="AE46">
         <f t="shared" si="14"/>
-        <v>1.4065626676239007</v>
+        <v>1.4062516797615263</v>
       </c>
       <c r="AF46">
         <f t="shared" si="15"/>
-        <v>1.278693334203546</v>
+        <v>1.2784106179650239</v>
       </c>
       <c r="AG46">
         <f t="shared" si="16"/>
@@ -6339,13 +6339,13 @@
         <v>-1</v>
       </c>
       <c r="M47">
-        <v>0.142481818351506</v>
+        <v>0.14245374033760591</v>
       </c>
       <c r="N47">
-        <v>3.0424433723253999E-2</v>
+        <v>3.041570759384463E-2</v>
       </c>
       <c r="O47">
-        <v>1.3535033916208699E-2</v>
+        <v>1.352298998064932E-2</v>
       </c>
       <c r="P47">
         <v>0.99639999999999995</v>
@@ -6404,15 +6404,15 @@
       </c>
       <c r="AD47">
         <f t="shared" si="13"/>
-        <v>0.70488079491707756</v>
+        <v>0.70471709350121003</v>
       </c>
       <c r="AE47">
         <f t="shared" si="14"/>
-        <v>1.4994852464442991</v>
+        <v>1.4991651287429271</v>
       </c>
       <c r="AF47">
         <f t="shared" si="15"/>
-        <v>1.3388261128966956</v>
+        <v>1.3385402935204704</v>
       </c>
       <c r="AG47">
         <f t="shared" si="16"/>
@@ -6454,13 +6454,13 @@
         <v>-1</v>
       </c>
       <c r="M48">
-        <v>0.14513434517395801</v>
+        <v>0.14510895432927451</v>
       </c>
       <c r="N48">
-        <v>4.2849076514962801E-2</v>
+        <v>4.2838881359871218E-2</v>
       </c>
       <c r="O48">
-        <v>1.3573172602199E-2</v>
+        <v>1.356181811587258E-2</v>
       </c>
       <c r="P48">
         <v>0.99639999999999995</v>
@@ -6519,15 +6519,15 @@
       </c>
       <c r="AD48">
         <f t="shared" si="13"/>
-        <v>0.79460445152722148</v>
+        <v>0.79444803524171692</v>
       </c>
       <c r="AE48">
         <f t="shared" si="14"/>
-        <v>1.5494314514838101</v>
+        <v>1.5491482278230317</v>
       </c>
       <c r="AF48">
         <f t="shared" si="15"/>
-        <v>1.3591503960384301</v>
+        <v>1.3589019542307297</v>
       </c>
       <c r="AG48">
         <f t="shared" si="16"/>
@@ -6569,13 +6569,13 @@
         <v>-1</v>
       </c>
       <c r="M49">
-        <v>0.127234019741681</v>
+        <v>0.12721773263294381</v>
       </c>
       <c r="N49">
-        <v>3.5851967777382497E-2</v>
+        <v>3.5845525684560307E-2</v>
       </c>
       <c r="O49">
-        <v>1.4689218305415599E-2</v>
+        <v>1.4678586021885711E-2</v>
       </c>
       <c r="P49">
         <v>0.99639999999999995</v>
@@ -6634,15 +6634,15 @@
       </c>
       <c r="AD49">
         <f t="shared" si="13"/>
-        <v>0.75482699995658875</v>
+        <v>0.75470019258131471</v>
       </c>
       <c r="AE49">
         <f t="shared" si="14"/>
-        <v>1.4629231082446013</v>
+        <v>1.4626206628621323</v>
       </c>
       <c r="AF49">
         <f t="shared" si="15"/>
-        <v>1.3061813466469654</v>
+        <v>1.3059113061269036</v>
       </c>
       <c r="AG49">
         <f t="shared" si="16"/>
@@ -6684,13 +6684,13 @@
         <v>-1</v>
       </c>
       <c r="M50">
-        <v>0.129732342503522</v>
+        <v>0.1297080758049812</v>
       </c>
       <c r="N50">
-        <v>3.7862025796940597E-2</v>
+        <v>3.7853696376787968E-2</v>
       </c>
       <c r="O50">
-        <v>7.7340636768012498E-3</v>
+        <v>7.7229371306208744E-3</v>
       </c>
       <c r="P50">
         <v>0.99639999999999995</v>
@@ -6749,15 +6749,15 @@
       </c>
       <c r="AD50">
         <f t="shared" si="13"/>
-        <v>0.70809610828801239</v>
+        <v>0.70792047028081762</v>
       </c>
       <c r="AE50">
         <f t="shared" si="14"/>
-        <v>1.4260103805422437</v>
+        <v>1.4256724086006716</v>
       </c>
       <c r="AF50">
         <f t="shared" si="15"/>
-        <v>1.3203799819835589</v>
+        <v>1.3200670450006218</v>
       </c>
       <c r="AG50">
         <f t="shared" si="16"/>
@@ -6797,13 +6797,13 @@
         <v>-1</v>
       </c>
       <c r="M51">
-        <v>0.12714845522482099</v>
+        <v>0.12712747278989411</v>
       </c>
       <c r="N51">
-        <v>3.4462391248614999E-2</v>
+        <v>3.4454418663742929E-2</v>
       </c>
       <c r="O51">
-        <v>1.13635874960701E-2</v>
+        <v>1.1351597884791131E-2</v>
       </c>
       <c r="P51">
         <v>0.99639999999999995</v>
@@ -6862,15 +6862,15 @@
       </c>
       <c r="AD51">
         <f t="shared" si="13"/>
-        <v>0.71791427225423132</v>
+        <v>0.71775193831985407</v>
       </c>
       <c r="AE51" s="1">
         <f t="shared" si="14"/>
-        <v>0.71791427225423132</v>
+        <v>0.71775193831985407</v>
       </c>
       <c r="AF51" s="1">
         <f t="shared" si="15"/>
-        <v>-2.5367995486015239E-2</v>
+        <v>-2.5362259304588481E-2</v>
       </c>
       <c r="AG51">
         <f t="shared" si="16"/>
@@ -6956,11 +6956,11 @@
       </c>
       <c r="AE52" s="1">
         <f t="shared" si="14"/>
-        <v>0.50455350742054139</v>
+        <v>0.49415931157930315</v>
       </c>
       <c r="AF52" s="1">
         <f t="shared" si="15"/>
-        <v>-1.7494920506953584E-2</v>
+        <v>-1.7134511497201913E-2</v>
       </c>
       <c r="AG52" s="1">
         <f t="shared" si="16"/>
@@ -6990,7 +6990,7 @@
         <v>61</v>
       </c>
       <c r="H53">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I53">
         <v>88</v>
@@ -7002,20 +7002,20 @@
         <v>-1</v>
       </c>
       <c r="M53">
-        <v>6.5962147204201793E-2</v>
+        <v>6.2107080403130913E-2</v>
       </c>
       <c r="N53">
-        <v>8.4226470710993002E-3</v>
+        <v>7.7431069869643224E-3</v>
       </c>
       <c r="O53">
-        <v>1.7606351476423102E-2</v>
+        <v>1.7637513061533949E-2</v>
       </c>
       <c r="P53">
         <v>0.99639999999999995</v>
       </c>
       <c r="Q53">
         <f t="shared" si="0"/>
-        <v>0.66</v>
+        <v>0.64</v>
       </c>
       <c r="R53">
         <f t="shared" si="1"/>
@@ -7035,15 +7035,15 @@
       </c>
       <c r="V53">
         <f t="shared" si="5"/>
-        <v>0.08</v>
+        <v>0.1</v>
       </c>
       <c r="W53">
         <f t="shared" si="6"/>
-        <v>0.24</v>
+        <v>0.26</v>
       </c>
       <c r="X53">
         <f t="shared" si="7"/>
-        <v>0.5</v>
+        <v>0.48</v>
       </c>
       <c r="Y53" s="2">
         <f>MEDIAN($U$53:$U$82)</f>
@@ -7067,19 +7067,19 @@
       </c>
       <c r="AD53">
         <f t="shared" si="13"/>
-        <v>0.50455350742054139</v>
+        <v>0.49415931157930315</v>
       </c>
       <c r="AE53">
         <f t="shared" si="14"/>
-        <v>1.0019631913421958</v>
+        <v>1.0250005430007738</v>
       </c>
       <c r="AF53">
         <f t="shared" si="15"/>
-        <v>0.78278374323609046</v>
+        <v>0.80078167421935453</v>
       </c>
       <c r="AG53">
         <f t="shared" si="16"/>
-        <v>90.909090909090907</v>
+        <v>93.75</v>
       </c>
     </row>
     <row r="54" spans="1:33" x14ac:dyDescent="0.2">
@@ -7096,7 +7096,7 @@
         <v>28</v>
       </c>
       <c r="E54">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F54">
         <v>61</v>
@@ -7117,28 +7117,28 @@
         <v>-1</v>
       </c>
       <c r="M54">
-        <v>6.15329772677361E-2</v>
+        <v>6.4652746977958073E-2</v>
       </c>
       <c r="N54">
-        <v>1.9835967517638099E-2</v>
+        <v>1.948685169647587E-2</v>
       </c>
       <c r="O54">
-        <v>2.9621364165086398E-3</v>
+        <v>5.5156724526434281E-3</v>
       </c>
       <c r="P54">
         <v>0.99639999999999995</v>
       </c>
       <c r="Q54">
         <f t="shared" si="0"/>
-        <v>0.62</v>
+        <v>0.64</v>
       </c>
       <c r="R54">
         <f t="shared" si="1"/>
-        <v>1.22</v>
+        <v>1.24</v>
       </c>
       <c r="S54">
         <f t="shared" si="2"/>
-        <v>0.8</v>
+        <v>0.82</v>
       </c>
       <c r="T54">
         <f t="shared" si="3"/>
@@ -7146,7 +7146,7 @@
       </c>
       <c r="U54">
         <f t="shared" si="4"/>
-        <v>0.08</v>
+        <v>0.1</v>
       </c>
       <c r="V54">
         <f t="shared" si="5"/>
@@ -7154,7 +7154,7 @@
       </c>
       <c r="W54">
         <f t="shared" si="6"/>
-        <v>0.26</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="X54">
         <f t="shared" si="7"/>
@@ -7182,19 +7182,19 @@
       </c>
       <c r="AD54">
         <f t="shared" si="13"/>
-        <v>0.49740968392165452</v>
+        <v>0.53084123142147066</v>
       </c>
       <c r="AE54">
         <f t="shared" si="14"/>
-        <v>1.1964762609541384</v>
+        <v>1.2297974827250697</v>
       </c>
       <c r="AF54">
         <f t="shared" si="15"/>
-        <v>0.98071824668371999</v>
+        <v>0.99177216348795949</v>
       </c>
       <c r="AG54">
         <f t="shared" si="16"/>
-        <v>96.774193548387103</v>
+        <v>93.75</v>
       </c>
     </row>
     <row r="55" spans="1:33" x14ac:dyDescent="0.2">
@@ -7232,13 +7232,13 @@
         <v>-1</v>
       </c>
       <c r="M55">
-        <v>0.107701826539227</v>
+        <v>0.1076937075191754</v>
       </c>
       <c r="N55">
-        <v>3.3547855111956702E-2</v>
+        <v>3.3539251607943993E-2</v>
       </c>
       <c r="O55">
-        <v>1.0011602067496199E-2</v>
+        <v>1.0006634121021891E-2</v>
       </c>
       <c r="P55">
         <v>0.99639999999999995</v>
@@ -7297,15 +7297,15 @@
       </c>
       <c r="AD55">
         <f t="shared" si="13"/>
-        <v>0.69906657703248387</v>
+        <v>0.69895625130359906</v>
       </c>
       <c r="AE55">
         <f t="shared" si="14"/>
-        <v>1.4390313587731729</v>
+        <v>1.4387513839313351</v>
       </c>
       <c r="AF55">
         <f t="shared" si="15"/>
-        <v>1.2623082094501519</v>
+        <v>1.2620626174836274</v>
       </c>
       <c r="AG55">
         <f t="shared" si="16"/>
@@ -7347,13 +7347,13 @@
         <v>-1</v>
       </c>
       <c r="M56">
-        <v>0.135044728488632</v>
+        <v>0.13502297609274869</v>
       </c>
       <c r="N56">
-        <v>3.6930556063132398E-2</v>
+        <v>3.6921868709916643E-2</v>
       </c>
       <c r="O56">
-        <v>1.18454971694813E-2</v>
+        <v>1.1832732146252011E-2</v>
       </c>
       <c r="P56">
         <v>0.99639999999999995</v>
@@ -7412,15 +7412,15 @@
       </c>
       <c r="AD56">
         <f t="shared" si="13"/>
-        <v>0.73996478174068903</v>
+        <v>0.73979513262773611</v>
       </c>
       <c r="AE56">
         <f t="shared" si="14"/>
-        <v>1.5520780939281402</v>
+        <v>1.551771562871072</v>
       </c>
       <c r="AF56">
         <f t="shared" si="15"/>
-        <v>1.3857840124358394</v>
+        <v>1.3855103239920283</v>
       </c>
       <c r="AG56">
         <f t="shared" si="16"/>
@@ -7462,13 +7462,13 @@
         <v>-1</v>
       </c>
       <c r="M57">
-        <v>0.15538665757703801</v>
+        <v>0.15536808041602129</v>
       </c>
       <c r="N57">
-        <v>3.8797804081331398E-2</v>
+        <v>3.8789143921520768E-2</v>
       </c>
       <c r="O57">
-        <v>1.9941135079112899E-2</v>
+        <v>1.9929167050317109E-2</v>
       </c>
       <c r="P57">
         <v>0.99639999999999995</v>
@@ -7527,15 +7527,15 @@
       </c>
       <c r="AD57">
         <f t="shared" si="13"/>
-        <v>0.81211331218745109</v>
+        <v>0.81197643024333588</v>
       </c>
       <c r="AE57">
         <f t="shared" si="14"/>
-        <v>1.5540100038694682</v>
+        <v>1.553691756328222</v>
       </c>
       <c r="AF57">
         <f t="shared" si="15"/>
-        <v>1.3875089320263108</v>
+        <v>1.3872247824359123</v>
       </c>
       <c r="AG57">
         <f t="shared" si="16"/>
@@ -7577,13 +7577,13 @@
         <v>-1</v>
       </c>
       <c r="M58">
-        <v>0.13925570386989899</v>
+        <v>0.13922579761608231</v>
       </c>
       <c r="N58">
-        <v>3.4980146081149202E-2</v>
+        <v>3.4966333350656027E-2</v>
       </c>
       <c r="O58">
-        <v>1.3830878140100001E-2</v>
+        <v>1.382060495744169E-2</v>
       </c>
       <c r="P58">
         <v>0.99639999999999995</v>
@@ -7642,15 +7642,15 @@
       </c>
       <c r="AD58">
         <f t="shared" si="13"/>
-        <v>0.74189669168201711</v>
+        <v>0.741715326084886</v>
       </c>
       <c r="AE58">
         <f t="shared" si="14"/>
-        <v>1.5471395504221594</v>
+        <v>1.5468540021899773</v>
       </c>
       <c r="AF58">
         <f t="shared" si="15"/>
-        <v>1.3813745985912136</v>
+        <v>1.3811196448124796</v>
       </c>
       <c r="AG58">
         <f t="shared" si="16"/>
@@ -7692,13 +7692,13 @@
         <v>-1</v>
       </c>
       <c r="M59">
-        <v>0.14725596605886801</v>
+        <v>0.14726797198657371</v>
       </c>
       <c r="N59">
-        <v>3.5626511601924399E-2</v>
+        <v>3.5624881212172901E-2</v>
       </c>
       <c r="O59">
-        <v>2.2472375018454799E-2</v>
+        <v>2.2457000999114209E-2</v>
       </c>
       <c r="P59">
         <v>0.99639999999999995</v>
@@ -7757,15 +7757,15 @@
       </c>
       <c r="AD59">
         <f t="shared" si="13"/>
-        <v>0.80524285874014234</v>
+        <v>0.80513867610509138</v>
       </c>
       <c r="AE59">
         <f t="shared" si="14"/>
-        <v>1.5892823366072426</v>
+        <v>1.5889951210475179</v>
       </c>
       <c r="AF59">
         <f t="shared" si="15"/>
-        <v>1.4190020862564665</v>
+        <v>1.4187456437924266</v>
       </c>
       <c r="AG59">
         <f t="shared" si="16"/>
@@ -7807,13 +7807,13 @@
         <v>-1</v>
       </c>
       <c r="M60">
-        <v>0.14311476749915999</v>
+        <v>0.14308287480228471</v>
       </c>
       <c r="N60">
-        <v>3.8051439111419498E-2</v>
+        <v>3.8040651425864727E-2</v>
       </c>
       <c r="O60">
-        <v>1.6541303143282001E-2</v>
+        <v>1.652614883852398E-2</v>
       </c>
       <c r="P60">
         <v>0.99639999999999995</v>
@@ -7872,15 +7872,15 @@
       </c>
       <c r="AD60">
         <f t="shared" si="13"/>
-        <v>0.78403947786710027</v>
+        <v>0.78385644494242668</v>
       </c>
       <c r="AE60">
         <f t="shared" si="14"/>
-        <v>1.6116976778313583</v>
+        <v>1.6113826423222157</v>
       </c>
       <c r="AF60">
         <f t="shared" si="15"/>
-        <v>1.413769892834525</v>
+        <v>1.4134935458966806</v>
       </c>
       <c r="AG60">
         <f t="shared" si="16"/>
@@ -7922,13 +7922,13 @@
         <v>-1</v>
       </c>
       <c r="M61">
-        <v>0.156848022582605</v>
+        <v>0.15682941604134781</v>
       </c>
       <c r="N61">
-        <v>4.0300401926473203E-2</v>
+        <v>4.0291205417550463E-2</v>
       </c>
       <c r="O61">
-        <v>2.0761933116235299E-2</v>
+        <v>2.0750872968281441E-2</v>
       </c>
       <c r="P61">
         <v>0.99639999999999995</v>
@@ -7987,15 +7987,15 @@
       </c>
       <c r="AD61">
         <f t="shared" si="13"/>
-        <v>0.82765819996425805</v>
+        <v>0.82752619737978894</v>
       </c>
       <c r="AE61">
         <f t="shared" si="14"/>
-        <v>1.5526731920666932</v>
+        <v>1.5523752925105909</v>
       </c>
       <c r="AF61">
         <f t="shared" si="15"/>
-        <v>1.3385113724712874</v>
+        <v>1.3382545625091302</v>
       </c>
       <c r="AG61">
         <f t="shared" si="16"/>
@@ -8037,13 +8037,13 @@
         <v>-1</v>
       </c>
       <c r="M62">
-        <v>0.11439033580709999</v>
+        <v>0.1143663456623131</v>
       </c>
       <c r="N62">
-        <v>4.1131107364451698E-2</v>
+        <v>4.1119698725027791E-2</v>
       </c>
       <c r="O62">
-        <v>7.20947185621527E-3</v>
+        <v>7.2013065588050051E-3</v>
       </c>
       <c r="P62">
         <v>0.99639999999999995</v>
@@ -8102,15 +8102,15 @@
       </c>
       <c r="AD62">
         <f t="shared" si="13"/>
-        <v>0.72501499210243503</v>
+        <v>0.72484909513080209</v>
       </c>
       <c r="AE62">
         <f t="shared" si="14"/>
-        <v>1.4269099449418907</v>
+        <v>1.4265696623536255</v>
       </c>
       <c r="AF62">
         <f t="shared" si="15"/>
-        <v>1.2971908590380823</v>
+        <v>1.2968815112305685</v>
       </c>
       <c r="AG62">
         <f t="shared" si="16"/>
@@ -8152,13 +8152,13 @@
         <v>-1</v>
       </c>
       <c r="M63">
-        <v>0.13045466968543401</v>
+        <v>0.13042819631232061</v>
       </c>
       <c r="N63">
-        <v>3.0678283353307498E-2</v>
+        <v>3.0670207867597839E-2</v>
       </c>
       <c r="O63">
-        <v>1.2908233115879899E-2</v>
+        <v>1.289448684133474E-2</v>
       </c>
       <c r="P63">
         <v>0.99639999999999995</v>
@@ -8217,15 +8217,15 @@
       </c>
       <c r="AD63">
         <f t="shared" si="13"/>
-        <v>0.7018949528394558</v>
+        <v>0.7017205672228235</v>
       </c>
       <c r="AE63">
         <f t="shared" si="14"/>
-        <v>1.4317541567468774</v>
+        <v>1.4314319219941021</v>
       </c>
       <c r="AF63">
         <f t="shared" si="15"/>
-        <v>1.3256982932841457</v>
+        <v>1.3253999277723167</v>
       </c>
       <c r="AG63">
         <f t="shared" si="16"/>
@@ -8267,13 +8267,13 @@
         <v>-1</v>
       </c>
       <c r="M64">
-        <v>0.12022258249275</v>
+        <v>0.12019955988231221</v>
       </c>
       <c r="N64">
-        <v>3.3360202691655801E-2</v>
+        <v>3.3351833180403627E-2</v>
       </c>
       <c r="O64">
-        <v>1.38326786488623E-2</v>
+        <v>1.382177080112903E-2</v>
       </c>
       <c r="P64">
         <v>0.99639999999999995</v>
@@ -8332,15 +8332,15 @@
       </c>
       <c r="AD64">
         <f t="shared" si="13"/>
-        <v>0.72985920390742176</v>
+        <v>0.72971135477127858</v>
       </c>
       <c r="AE64">
         <f t="shared" si="14"/>
-        <v>1.5439864574578426</v>
+        <v>1.5437279351747069</v>
       </c>
       <c r="AF64">
         <f t="shared" si="15"/>
-        <v>1.3543740854893358</v>
+        <v>1.3541473115567606</v>
       </c>
       <c r="AG64">
         <f t="shared" si="16"/>
@@ -8382,13 +8382,13 @@
         <v>-1</v>
       </c>
       <c r="M65">
-        <v>0.14972242734958499</v>
+        <v>0.14969304567415909</v>
       </c>
       <c r="N65">
-        <v>3.90215693658355E-2</v>
+        <v>3.9014784504160661E-2</v>
       </c>
       <c r="O65">
-        <v>2.0013024773171299E-2</v>
+        <v>2.000307037827586E-2</v>
       </c>
       <c r="P65">
         <v>0.99639999999999995</v>
@@ -8447,15 +8447,15 @@
       </c>
       <c r="AD65">
         <f t="shared" si="13"/>
-        <v>0.8141272535504207</v>
+        <v>0.81401658040342828</v>
       </c>
       <c r="AE65">
         <f t="shared" si="14"/>
-        <v>1.5126955479613096</v>
+        <v>1.5125103008762553</v>
       </c>
       <c r="AF65">
         <f t="shared" si="15"/>
-        <v>1.3269259192643068</v>
+        <v>1.3267634218212767</v>
       </c>
       <c r="AG65">
         <f t="shared" si="16"/>
@@ -8497,13 +8497,13 @@
         <v>-1</v>
       </c>
       <c r="M66">
-        <v>0.121192250805538</v>
+        <v>0.1211373526726867</v>
       </c>
       <c r="N66">
-        <v>3.24663103031003E-2</v>
+        <v>3.2448886232079428E-2</v>
       </c>
       <c r="O66">
-        <v>1.08664332719247E-2</v>
+        <v>1.0873081640722281E-2</v>
       </c>
       <c r="P66">
         <v>0.99639999999999995</v>
@@ -8562,15 +8562,15 @@
       </c>
       <c r="AD66">
         <f t="shared" si="13"/>
-        <v>0.69856829441088886</v>
+        <v>0.6984937204728271</v>
       </c>
       <c r="AE66">
         <f t="shared" si="14"/>
-        <v>1.5100349340516246</v>
+        <v>1.5098028376814918</v>
       </c>
       <c r="AF66">
         <f t="shared" si="15"/>
-        <v>1.3482454768318075</v>
+        <v>1.3480382479299033</v>
       </c>
       <c r="AG66">
         <f t="shared" si="16"/>
@@ -8612,13 +8612,13 @@
         <v>-1</v>
       </c>
       <c r="M67">
-        <v>0.13420620945395101</v>
+        <v>0.13418602001070301</v>
       </c>
       <c r="N67">
-        <v>4.0531239420579998E-2</v>
+        <v>4.0520789006815057E-2</v>
       </c>
       <c r="O67">
-        <v>1.8030303278540001E-2</v>
+        <v>1.801750420916998E-2</v>
       </c>
       <c r="P67">
         <v>0.99639999999999995</v>
@@ -8677,15 +8677,15 @@
       </c>
       <c r="AD67">
         <f t="shared" ref="AD67:AD81" si="30">2 * SQRT(2 * P67 * N67 - N67 * N67) + 2 * SQRT(2 * AC67 * O67 - O67 * O67)</f>
-        <v>0.81146663964073573</v>
+        <v>0.81130911720866483</v>
       </c>
       <c r="AE67">
         <f t="shared" ref="AE67:AE80" si="31">AD67+AD68</f>
-        <v>1.5118191282594173</v>
+        <v>1.5114450492392431</v>
       </c>
       <c r="AF67">
         <f t="shared" ref="AF67:AF80" si="32">AE67/R67</f>
-        <v>1.3498385073744796</v>
+        <v>1.349504508249324</v>
       </c>
       <c r="AG67">
         <f t="shared" ref="AG67:AG81" si="33">60/Q67</f>
@@ -8727,13 +8727,13 @@
         <v>-1</v>
       </c>
       <c r="M68">
-        <v>0.131431722588325</v>
+        <v>0.13140982248765881</v>
       </c>
       <c r="N68">
-        <v>3.1844251657882801E-2</v>
+        <v>3.183400787845439E-2</v>
       </c>
       <c r="O68">
-        <v>1.16241057930667E-2</v>
+        <v>1.16079605870174E-2</v>
       </c>
       <c r="P68">
         <v>0.99639999999999995</v>
@@ -8792,15 +8792,15 @@
       </c>
       <c r="AD68">
         <f t="shared" si="30"/>
-        <v>0.70035248861868149</v>
+        <v>0.70013593203057811</v>
       </c>
       <c r="AE68">
         <f t="shared" si="31"/>
-        <v>1.5348784023949444</v>
+        <v>1.534504003149582</v>
       </c>
       <c r="AF68">
         <f t="shared" si="32"/>
-        <v>1.3463845635043374</v>
+        <v>1.3460561431136686</v>
       </c>
       <c r="AG68">
         <f t="shared" si="33"/>
@@ -8842,13 +8842,13 @@
         <v>-1</v>
       </c>
       <c r="M69">
-        <v>0.142893896165429</v>
+        <v>0.14286872369859621</v>
       </c>
       <c r="N69">
-        <v>4.4678071253246902E-2</v>
+        <v>4.4668908084003242E-2</v>
       </c>
       <c r="O69">
-        <v>1.7386449401944601E-2</v>
+        <v>1.7372121523746311E-2</v>
       </c>
       <c r="P69">
         <v>0.99639999999999995</v>
@@ -8907,15 +8907,15 @@
       </c>
       <c r="AD69">
         <f t="shared" si="30"/>
-        <v>0.83452591377626284</v>
+        <v>0.8343680711190038</v>
       </c>
       <c r="AE69">
         <f t="shared" si="31"/>
-        <v>1.5467057227589025</v>
+        <v>1.5465556557583735</v>
       </c>
       <c r="AF69">
         <f t="shared" si="32"/>
-        <v>1.3333670023783644</v>
+        <v>1.3332376342744601</v>
       </c>
       <c r="AG69">
         <f t="shared" si="33"/>
@@ -8957,13 +8957,13 @@
         <v>-1</v>
       </c>
       <c r="M70">
-        <v>0.12869684579014801</v>
+        <v>0.12866673521666841</v>
       </c>
       <c r="N70">
-        <v>3.5263169400284497E-2</v>
+        <v>3.525154083180565E-2</v>
       </c>
       <c r="O70">
-        <v>1.0054946196745299E-2</v>
+        <v>1.006506800715371E-2</v>
       </c>
       <c r="P70">
         <v>0.99639999999999995</v>
@@ -9022,15 +9022,15 @@
       </c>
       <c r="AD70">
         <f t="shared" si="30"/>
-        <v>0.71217980898263966</v>
+        <v>0.71218758463936971</v>
       </c>
       <c r="AE70">
         <f t="shared" si="31"/>
-        <v>1.4196718152453724</v>
+        <v>1.4194886969447933</v>
       </c>
       <c r="AF70">
         <f t="shared" si="32"/>
-        <v>1.2675641207547967</v>
+        <v>1.2674006222721368</v>
       </c>
       <c r="AG70">
         <f t="shared" si="33"/>
@@ -9072,13 +9072,13 @@
         <v>-1</v>
       </c>
       <c r="M71">
-        <v>0.118244330269601</v>
+        <v>0.11822820641636381</v>
       </c>
       <c r="N71">
-        <v>3.2941351010035799E-2</v>
+        <v>3.2933057518627698E-2</v>
       </c>
       <c r="O71">
-        <v>1.1477191814527801E-2</v>
+        <v>1.146225823519802E-2</v>
       </c>
       <c r="P71">
         <v>0.99639999999999995</v>
@@ -9137,15 +9137,15 @@
       </c>
       <c r="AD71">
         <f t="shared" si="30"/>
-        <v>0.70749200626273279</v>
+        <v>0.70730111230542358</v>
       </c>
       <c r="AE71">
         <f t="shared" si="31"/>
-        <v>1.4304395166389632</v>
+        <v>1.4300655192468517</v>
       </c>
       <c r="AF71">
         <f t="shared" si="32"/>
-        <v>1.277178139856217</v>
+        <v>1.2768442136132603</v>
       </c>
       <c r="AG71">
         <f t="shared" si="33"/>
@@ -9187,13 +9187,13 @@
         <v>-1</v>
       </c>
       <c r="M72">
-        <v>0.13604713517748299</v>
+        <v>0.13601709572229481</v>
       </c>
       <c r="N72">
-        <v>3.68726021258707E-2</v>
+        <v>3.6863434730021127E-2</v>
       </c>
       <c r="O72">
-        <v>9.9604932634023008E-3</v>
+        <v>9.9477462999892005E-3</v>
       </c>
       <c r="P72">
         <v>0.99639999999999995</v>
@@ -9252,15 +9252,15 @@
       </c>
       <c r="AD72">
         <f t="shared" si="30"/>
-        <v>0.7229475103762304</v>
+        <v>0.72276440694142807</v>
       </c>
       <c r="AE72">
         <f t="shared" si="31"/>
-        <v>1.4776414764089609</v>
+        <v>1.4772016015091252</v>
       </c>
       <c r="AF72">
         <f t="shared" si="32"/>
-        <v>1.319322746793715</v>
+        <v>1.318930001347433</v>
       </c>
       <c r="AG72">
         <f t="shared" si="33"/>
@@ -9302,13 +9302,13 @@
         <v>-1</v>
       </c>
       <c r="M73">
-        <v>0.13581413447052201</v>
+        <v>0.13577276596830001</v>
       </c>
       <c r="N73">
-        <v>3.5471747001121802E-2</v>
+        <v>3.5453481333852038E-2</v>
       </c>
       <c r="O73">
-        <v>1.5040968064534499E-2</v>
+        <v>1.5024363537944689E-2</v>
       </c>
       <c r="P73">
         <v>0.99639999999999995</v>
@@ -9367,15 +9367,15 @@
       </c>
       <c r="AD73">
         <f t="shared" si="30"/>
-        <v>0.75469396603273065</v>
+        <v>0.7544371945676972</v>
       </c>
       <c r="AE73">
         <f t="shared" si="31"/>
-        <v>1.4598690343868554</v>
+        <v>1.4594489057593152</v>
       </c>
       <c r="AF73">
         <f t="shared" si="32"/>
-        <v>1.3034544949882636</v>
+        <v>1.3030793801422456</v>
       </c>
       <c r="AG73">
         <f t="shared" si="33"/>
@@ -9417,13 +9417,13 @@
         <v>-1</v>
       </c>
       <c r="M74">
-        <v>0.124667355986653</v>
+        <v>0.1246433571219311</v>
       </c>
       <c r="N74">
-        <v>2.94615441309336E-2</v>
+        <v>2.9451984676048749E-2</v>
       </c>
       <c r="O74">
-        <v>1.45690379610947E-2</v>
+        <v>1.455760540092664E-2</v>
       </c>
       <c r="P74">
         <v>0.99639999999999995</v>
@@ -9482,15 +9482,15 @@
       </c>
       <c r="AD74">
         <f t="shared" si="30"/>
-        <v>0.70517506835412491</v>
+        <v>0.70501171119161798</v>
       </c>
       <c r="AE74">
         <f t="shared" si="31"/>
-        <v>1.5213402433534111</v>
+        <v>1.5210456653108151</v>
       </c>
       <c r="AF74">
         <f t="shared" si="32"/>
-        <v>1.2892713926723824</v>
+        <v>1.2890217502634027</v>
       </c>
       <c r="AG74">
         <f t="shared" si="33"/>
@@ -9532,13 +9532,13 @@
         <v>-1</v>
       </c>
       <c r="M75">
-        <v>0.137911711644539</v>
+        <v>0.1379038097797379</v>
       </c>
       <c r="N75">
-        <v>4.0419319280604098E-2</v>
+        <v>4.0409767234049918E-2</v>
       </c>
       <c r="O75">
-        <v>1.8848016341235199E-2</v>
+        <v>1.883798491645251E-2</v>
       </c>
       <c r="P75">
         <v>0.99639999999999995</v>
@@ -9597,15 +9597,15 @@
       </c>
       <c r="AD75">
         <f t="shared" si="30"/>
-        <v>0.81616517499928631</v>
+        <v>0.8160339541191971</v>
       </c>
       <c r="AE75">
         <f t="shared" si="31"/>
-        <v>1.5348783293280759</v>
+        <v>1.5347584860823664</v>
       </c>
       <c r="AF75">
         <f t="shared" si="32"/>
-        <v>1.3007443468882001</v>
+        <v>1.3006427848155648</v>
       </c>
       <c r="AG75">
         <f t="shared" si="33"/>
@@ -9647,13 +9647,13 @@
         <v>-1</v>
       </c>
       <c r="M76">
-        <v>0.122122974052674</v>
+        <v>0.1220754468041173</v>
       </c>
       <c r="N76">
-        <v>3.25011412294249E-2</v>
+        <v>3.248775217753018E-2</v>
       </c>
       <c r="O76">
-        <v>1.32436790142607E-2</v>
+        <v>1.325797603085988E-2</v>
       </c>
       <c r="P76">
         <v>0.99639999999999995</v>
@@ -9712,15 +9712,15 @@
       </c>
       <c r="AD76">
         <f t="shared" si="30"/>
-        <v>0.71871315432878946</v>
+        <v>0.71872453196316932</v>
       </c>
       <c r="AE76">
         <f t="shared" si="31"/>
-        <v>1.4557929572591659</v>
+        <v>1.4555944028414216</v>
       </c>
       <c r="AF76">
         <f t="shared" si="32"/>
-        <v>1.2998151404099694</v>
+        <v>1.2996378596798406</v>
       </c>
       <c r="AG76">
         <f t="shared" si="33"/>
@@ -9762,13 +9762,13 @@
         <v>-1</v>
       </c>
       <c r="M77">
-        <v>0.13920599561528699</v>
+        <v>0.1391753332108133</v>
       </c>
       <c r="N77">
-        <v>3.32973193586188E-2</v>
+        <v>3.328548894165332E-2</v>
       </c>
       <c r="O77">
-        <v>1.48413398113193E-2</v>
+        <v>1.482522772407893E-2</v>
       </c>
       <c r="P77">
         <v>0.99639999999999995</v>
@@ -9827,15 +9827,15 @@
       </c>
       <c r="AD77">
         <f t="shared" si="30"/>
-        <v>0.73707980293037634</v>
+        <v>0.7368698708782524</v>
       </c>
       <c r="AE77">
         <f t="shared" si="31"/>
-        <v>1.5367868237251483</v>
+        <v>1.5363920852330184</v>
       </c>
       <c r="AF77">
         <f t="shared" si="32"/>
-        <v>1.3248162273492659</v>
+        <v>1.3244759355457056</v>
       </c>
       <c r="AG77">
         <f t="shared" si="33"/>
@@ -9877,13 +9877,13 @@
         <v>-1</v>
       </c>
       <c r="M78">
-        <v>0.13916227688779501</v>
+        <v>0.13914691482014149</v>
       </c>
       <c r="N78">
-        <v>4.3187774607578097E-2</v>
+        <v>4.3174540151220048E-2</v>
       </c>
       <c r="O78">
-        <v>1.3941721479900001E-2</v>
+        <v>1.3929082626169761E-2</v>
       </c>
       <c r="P78">
         <v>0.99639999999999995</v>
@@ -9942,15 +9942,15 @@
       </c>
       <c r="AD78">
         <f t="shared" si="30"/>
-        <v>0.79970702079477207</v>
+        <v>0.799522214354766</v>
       </c>
       <c r="AE78">
         <f t="shared" si="31"/>
-        <v>1.4890899819665018</v>
+        <v>1.4887050978403482</v>
       </c>
       <c r="AF78">
         <f t="shared" si="32"/>
-        <v>1.2836982603159499</v>
+        <v>1.2833664636554727</v>
       </c>
       <c r="AG78">
         <f t="shared" si="33"/>
@@ -9992,13 +9992,13 @@
         <v>-1</v>
       </c>
       <c r="M79">
-        <v>0.118257344868237</v>
+        <v>0.1182391296372536</v>
       </c>
       <c r="N79">
-        <v>3.1964239639497703E-2</v>
+        <v>3.195118832892789E-2</v>
       </c>
       <c r="O79">
-        <v>1.02701837653736E-2</v>
+        <v>1.025922349771159E-2</v>
       </c>
       <c r="P79">
         <v>0.99639999999999995</v>
@@ -10057,15 +10057,15 @@
       </c>
       <c r="AD79">
         <f t="shared" si="30"/>
-        <v>0.68938296117172959</v>
+        <v>0.68918288348558221</v>
       </c>
       <c r="AE79">
         <f t="shared" si="31"/>
-        <v>1.412437442102068</v>
+        <v>1.4120429843824072</v>
       </c>
       <c r="AF79">
         <f t="shared" si="32"/>
-        <v>1.2611048590197034</v>
+        <v>1.2607526646271492</v>
       </c>
       <c r="AG79">
         <f t="shared" si="33"/>
@@ -10107,13 +10107,13 @@
         <v>-1</v>
       </c>
       <c r="M80">
-        <v>0.133639249375099</v>
+        <v>0.13362955863584891</v>
       </c>
       <c r="N80">
-        <v>3.5827480105498799E-2</v>
+        <v>3.581403478087114E-2</v>
       </c>
       <c r="O80">
-        <v>1.08059352597581E-2</v>
+        <v>1.079498643469433E-2</v>
       </c>
       <c r="P80">
         <v>0.99639999999999995</v>
@@ -10172,15 +10172,15 @@
       </c>
       <c r="AD80">
         <f t="shared" si="30"/>
-        <v>0.72305448093033853</v>
+        <v>0.72286010089682506</v>
       </c>
       <c r="AE80">
         <f t="shared" si="31"/>
-        <v>1.5175238329758616</v>
+        <v>1.5172406323764474</v>
       </c>
       <c r="AF80">
         <f t="shared" si="32"/>
-        <v>1.3549319937284476</v>
+        <v>1.3546791360503994</v>
       </c>
       <c r="AG80">
         <f t="shared" si="33"/>
@@ -10220,13 +10220,13 @@
         <v>-1</v>
       </c>
       <c r="M81">
-        <v>0.12618727408369701</v>
+        <v>0.12620143733849351</v>
       </c>
       <c r="N81">
-        <v>3.7998229092669297E-2</v>
+        <v>3.7998304872406248E-2</v>
       </c>
       <c r="O81">
-        <v>1.8106276975441801E-2</v>
+        <v>1.8093025341240611E-2</v>
       </c>
       <c r="P81">
         <v>0.99639999999999995</v>
@@ -10279,7 +10279,7 @@
       </c>
       <c r="AD81">
         <f t="shared" si="30"/>
-        <v>0.79446935204552305</v>
+        <v>0.79438053147962218</v>
       </c>
       <c r="AE81" s="1"/>
       <c r="AF81" s="1"/>

</xml_diff>